<commit_message>
Agregar datos en carpeta de ventas inconsistentes
</commit_message>
<xml_diff>
--- a/Data/Temp/Reporte fidelizaciones Satelite.xlsx
+++ b/Data/Temp/Reporte fidelizaciones Satelite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPathProject\SBTT0044-Conciliacion-Terpel\Data\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robot.11\Documents\UiPath\Conciliacion EDS\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="281">
   <si>
     <t>No. Recibo sin PPC</t>
   </si>
@@ -865,6 +865,9 @@
   </si>
   <si>
     <t>109500</t>
+  </si>
+  <si>
+    <t>Validación</t>
   </si>
 </sst>
 </file>
@@ -907,9 +910,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,18 +1194,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:KEZ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="7591" width="11.453125" style="1"/>
+    <col min="7592" max="7592" width="11.453125" style="2"/>
+    <col min="7593" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,8 +1233,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="KEZ1" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1259,7 +1266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1288,7 +1295,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1317,7 +1324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1346,7 +1353,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1375,7 +1382,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1404,7 +1411,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1433,7 +1440,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1462,7 +1469,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1520,7 +1527,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -1578,7 +1585,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1607,7 +1614,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
@@ -1636,7 +1643,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
@@ -1665,7 +1672,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -1694,7 +1701,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -1723,7 +1730,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
@@ -1752,7 +1759,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
@@ -1781,7 +1788,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -1810,7 +1817,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>87</v>
       </c>
@@ -1839,7 +1846,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>93</v>
       </c>
@@ -1868,7 +1875,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>97</v>
       </c>
@@ -1897,7 +1904,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>100</v>
       </c>
@@ -1926,7 +1933,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>104</v>
       </c>
@@ -1955,7 +1962,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>107</v>
       </c>
@@ -1984,7 +1991,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>111</v>
       </c>
@@ -2013,7 +2020,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>114</v>
       </c>
@@ -2042,7 +2049,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>118</v>
       </c>
@@ -2071,7 +2078,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
@@ -2100,7 +2107,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>127</v>
       </c>
@@ -2129,7 +2136,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>130</v>
       </c>
@@ -2158,7 +2165,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>133</v>
       </c>
@@ -2187,7 +2194,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>136</v>
       </c>
@@ -2216,7 +2223,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>140</v>
       </c>
@@ -2245,7 +2252,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>144</v>
       </c>
@@ -2274,7 +2281,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>148</v>
       </c>
@@ -2303,7 +2310,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>151</v>
       </c>
@@ -2332,7 +2339,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>154</v>
       </c>
@@ -2361,7 +2368,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>157</v>
       </c>
@@ -2390,7 +2397,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>161</v>
       </c>
@@ -2419,7 +2426,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>164</v>
       </c>
@@ -2448,7 +2455,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>168</v>
       </c>
@@ -2477,7 +2484,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>172</v>
       </c>
@@ -2506,7 +2513,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>175</v>
       </c>
@@ -2535,7 +2542,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>179</v>
       </c>
@@ -2564,7 +2571,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>182</v>
       </c>
@@ -2593,7 +2600,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>186</v>
       </c>
@@ -2622,7 +2629,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>189</v>
       </c>
@@ -2651,7 +2658,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>193</v>
       </c>
@@ -2680,7 +2687,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>197</v>
       </c>
@@ -2709,7 +2716,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>200</v>
       </c>
@@ -2738,7 +2745,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>204</v>
       </c>
@@ -2767,7 +2774,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>207</v>
       </c>
@@ -2796,7 +2803,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>211</v>
       </c>
@@ -2825,7 +2832,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>215</v>
       </c>
@@ -2854,7 +2861,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>219</v>
       </c>
@@ -2883,7 +2890,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>222</v>
       </c>
@@ -2912,7 +2919,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>226</v>
       </c>
@@ -2941,7 +2948,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>230</v>
       </c>
@@ -2970,7 +2977,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>233</v>
       </c>
@@ -2999,7 +3006,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>237</v>
       </c>
@@ -3028,7 +3035,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>241</v>
       </c>
@@ -3057,7 +3064,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>244</v>
       </c>
@@ -3086,7 +3093,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="66" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>248</v>
       </c>
@@ -3115,7 +3122,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="67" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>251</v>
       </c>
@@ -3144,7 +3151,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>255</v>
       </c>
@@ -3173,7 +3180,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="69" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>259</v>
       </c>
@@ -3202,7 +3209,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>262</v>
       </c>
@@ -3231,7 +3238,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>266</v>
       </c>
@@ -3260,7 +3267,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="72" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>270</v>
       </c>
@@ -3289,7 +3296,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>273</v>
       </c>
@@ -3318,7 +3325,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>277</v>
       </c>
@@ -3359,7 +3366,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización del dia 07/04/2022
</commit_message>
<xml_diff>
--- a/Data/Temp/Reporte fidelizaciones Satelite.xlsx
+++ b/Data/Temp/Reporte fidelizaciones Satelite.xlsx
@@ -1194,9 +1194,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:KEZ74"/>
+  <dimension ref="A1:KEZ75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1238,40 +1240,16 @@
       </c>
     </row>
     <row r="2" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -1280,7 +1258,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -1292,15 +1270,15 @@
         <v>100000000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1309,7 +1287,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1321,15 +1299,15 @@
         <v>100000000</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -1338,7 +1316,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
@@ -1355,10 +1333,10 @@
     </row>
     <row r="6" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -1367,7 +1345,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
@@ -1379,15 +1357,15 @@
         <v>100000000</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
@@ -1396,7 +1374,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>14</v>
@@ -1408,15 +1386,15 @@
         <v>100000000</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
@@ -1425,7 +1403,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
@@ -1442,10 +1420,10 @@
     </row>
     <row r="9" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>11</v>
@@ -1454,7 +1432,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>14</v>
@@ -1463,18 +1441,18 @@
         <v>15</v>
       </c>
       <c r="H9" s="1">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -1483,7 +1461,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -1500,10 +1478,10 @@
     </row>
     <row r="11" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
@@ -1512,7 +1490,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>14</v>
@@ -1524,15 +1502,15 @@
         <v>150000000</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>11</v>
@@ -1541,7 +1519,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>14</v>
@@ -1550,18 +1528,18 @@
         <v>15</v>
       </c>
       <c r="H12" s="1">
-        <v>100000000</v>
+        <v>150000000</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
@@ -1570,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>14</v>
@@ -1582,15 +1560,15 @@
         <v>100000000</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
@@ -1599,7 +1577,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>14</v>
@@ -1611,15 +1589,15 @@
         <v>100000000</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
@@ -1628,7 +1606,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>14</v>
@@ -1645,10 +1623,10 @@
     </row>
     <row r="16" spans="1:9 7592:7592" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
@@ -1657,7 +1635,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>14</v>
@@ -1669,15 +1647,15 @@
         <v>100000000</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>11</v>
@@ -1686,7 +1664,7 @@
         <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>14</v>
@@ -1703,10 +1681,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>11</v>
@@ -1715,7 +1693,7 @@
         <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>14</v>
@@ -1727,15 +1705,15 @@
         <v>100000000</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>11</v>
@@ -1744,7 +1722,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -1753,18 +1731,18 @@
         <v>15</v>
       </c>
       <c r="H19" s="1">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>11</v>
@@ -1773,7 +1751,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>14</v>
@@ -1790,10 +1768,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>11</v>
@@ -1802,7 +1780,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>14</v>
@@ -1814,24 +1792,24 @@
         <v>150000000</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
@@ -1840,18 +1818,18 @@
         <v>15</v>
       </c>
       <c r="H22" s="1">
-        <v>100000000</v>
+        <v>150000000</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>89</v>
@@ -1860,7 +1838,7 @@
         <v>90</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
@@ -1872,15 +1850,15 @@
         <v>100000000</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>89</v>
@@ -1889,7 +1867,7 @@
         <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>14</v>
@@ -1906,10 +1884,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>89</v>
@@ -1918,7 +1896,7 @@
         <v>90</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>14</v>
@@ -1930,15 +1908,15 @@
         <v>100000000</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>89</v>
@@ -1947,7 +1925,7 @@
         <v>90</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>14</v>
@@ -1964,10 +1942,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>89</v>
@@ -1976,7 +1954,7 @@
         <v>90</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>14</v>
@@ -1988,15 +1966,15 @@
         <v>100000000</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>89</v>
@@ -2005,7 +1983,7 @@
         <v>90</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>14</v>
@@ -2014,7 +1992,7 @@
         <v>15</v>
       </c>
       <c r="H28" s="1">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>110</v>
@@ -2022,10 +2000,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>89</v>
@@ -2034,7 +2012,7 @@
         <v>90</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>14</v>
@@ -2043,18 +2021,18 @@
         <v>15</v>
       </c>
       <c r="H29" s="1">
-        <v>100000000</v>
+        <v>150000000</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>89</v>
@@ -2063,7 +2041,7 @@
         <v>90</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>14</v>
@@ -2080,19 +2058,19 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>14</v>
@@ -2104,15 +2082,15 @@
         <v>100000000</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>123</v>
@@ -2121,7 +2099,7 @@
         <v>124</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>14</v>
@@ -2138,10 +2116,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>123</v>
@@ -2150,7 +2128,7 @@
         <v>124</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>14</v>
@@ -2167,10 +2145,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>123</v>
@@ -2179,7 +2157,7 @@
         <v>124</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>14</v>
@@ -2196,10 +2174,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>123</v>
@@ -2208,7 +2186,7 @@
         <v>124</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>14</v>
@@ -2220,15 +2198,15 @@
         <v>100000000</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>123</v>
@@ -2237,7 +2215,7 @@
         <v>124</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>14</v>
@@ -2249,15 +2227,15 @@
         <v>100000000</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>123</v>
@@ -2266,7 +2244,7 @@
         <v>124</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>14</v>
@@ -2278,15 +2256,15 @@
         <v>100000000</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>123</v>
@@ -2295,7 +2273,7 @@
         <v>124</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -2304,7 +2282,7 @@
         <v>15</v>
       </c>
       <c r="H38" s="1">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>147</v>
@@ -2312,10 +2290,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>123</v>
@@ -2324,7 +2302,7 @@
         <v>124</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>14</v>
@@ -2341,10 +2319,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>123</v>
@@ -2353,7 +2331,7 @@
         <v>124</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>14</v>
@@ -2370,10 +2348,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>123</v>
@@ -2382,7 +2360,7 @@
         <v>124</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>14</v>
@@ -2391,18 +2369,18 @@
         <v>15</v>
       </c>
       <c r="H41" s="1">
-        <v>100000000</v>
+        <v>150000000</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>123</v>
@@ -2411,7 +2389,7 @@
         <v>124</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>14</v>
@@ -2428,10 +2406,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>123</v>
@@ -2440,7 +2418,7 @@
         <v>124</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>14</v>
@@ -2452,15 +2430,15 @@
         <v>100000000</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>123</v>
@@ -2469,7 +2447,7 @@
         <v>124</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>14</v>
@@ -2481,15 +2459,15 @@
         <v>100000000</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>123</v>
@@ -2498,7 +2476,7 @@
         <v>124</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>14</v>
@@ -2515,19 +2493,19 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>14</v>
@@ -2539,15 +2517,15 @@
         <v>100000000</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>89</v>
@@ -2556,7 +2534,7 @@
         <v>90</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>14</v>
@@ -2573,10 +2551,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>89</v>
@@ -2585,7 +2563,7 @@
         <v>90</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>14</v>
@@ -2597,15 +2575,15 @@
         <v>100000000</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>89</v>
@@ -2614,7 +2592,7 @@
         <v>90</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>14</v>
@@ -2631,10 +2609,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>89</v>
@@ -2643,7 +2621,7 @@
         <v>90</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>14</v>
@@ -2655,15 +2633,15 @@
         <v>100000000</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>89</v>
@@ -2672,7 +2650,7 @@
         <v>90</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>14</v>
@@ -2684,15 +2662,15 @@
         <v>100000000</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>89</v>
@@ -2701,7 +2679,7 @@
         <v>90</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>14</v>
@@ -2718,10 +2696,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>89</v>
@@ -2730,7 +2708,7 @@
         <v>90</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>14</v>
@@ -2742,15 +2720,15 @@
         <v>100000000</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>89</v>
@@ -2759,7 +2737,7 @@
         <v>90</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>14</v>
@@ -2776,10 +2754,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>89</v>
@@ -2788,7 +2766,7 @@
         <v>90</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>14</v>
@@ -2800,15 +2778,15 @@
         <v>100000000</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>89</v>
@@ -2817,7 +2795,7 @@
         <v>90</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>14</v>
@@ -2826,18 +2804,18 @@
         <v>15</v>
       </c>
       <c r="H56" s="1">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>89</v>
@@ -2846,7 +2824,7 @@
         <v>90</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>14</v>
@@ -2858,15 +2836,15 @@
         <v>150000000</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>89</v>
@@ -2875,7 +2853,7 @@
         <v>90</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>14</v>
@@ -2892,10 +2870,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>89</v>
@@ -2904,7 +2882,7 @@
         <v>90</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>14</v>
@@ -2913,18 +2891,18 @@
         <v>15</v>
       </c>
       <c r="H59" s="1">
-        <v>100000000</v>
+        <v>150000000</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>89</v>
@@ -2933,7 +2911,7 @@
         <v>90</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>14</v>
@@ -2945,15 +2923,15 @@
         <v>100000000</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>89</v>
@@ -2962,7 +2940,7 @@
         <v>90</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>14</v>
@@ -2979,19 +2957,19 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>14</v>
@@ -3003,15 +2981,15 @@
         <v>100000000</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>11</v>
@@ -3020,7 +2998,7 @@
         <v>12</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>14</v>
@@ -3032,15 +3010,15 @@
         <v>100000000</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -3049,7 +3027,7 @@
         <v>12</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>14</v>
@@ -3066,10 +3044,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
@@ -3078,7 +3056,7 @@
         <v>12</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>14</v>
@@ -3090,15 +3068,15 @@
         <v>100000000</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -3107,7 +3085,7 @@
         <v>12</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>14</v>
@@ -3124,10 +3102,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>11</v>
@@ -3136,7 +3114,7 @@
         <v>12</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>14</v>
@@ -3148,15 +3126,15 @@
         <v>100000000</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>11</v>
@@ -3165,7 +3143,7 @@
         <v>12</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>14</v>
@@ -3177,15 +3155,15 @@
         <v>100000000</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>11</v>
@@ -3194,7 +3172,7 @@
         <v>12</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>14</v>
@@ -3211,10 +3189,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>11</v>
@@ -3223,7 +3201,7 @@
         <v>12</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>14</v>
@@ -3235,15 +3213,15 @@
         <v>100000000</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>11</v>
@@ -3252,7 +3230,7 @@
         <v>12</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>14</v>
@@ -3261,18 +3239,18 @@
         <v>15</v>
       </c>
       <c r="H71" s="1">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>11</v>
@@ -3281,7 +3259,7 @@
         <v>12</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>14</v>
@@ -3290,7 +3268,7 @@
         <v>15</v>
       </c>
       <c r="H72" s="1">
-        <v>100000000</v>
+        <v>150000000</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>269</v>
@@ -3298,10 +3276,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>11</v>
@@ -3310,7 +3288,7 @@
         <v>12</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>14</v>
@@ -3319,18 +3297,18 @@
         <v>15</v>
       </c>
       <c r="H73" s="1">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>11</v>
@@ -3339,7 +3317,7 @@
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>14</v>
@@ -3351,6 +3329,35 @@
         <v>150000000</v>
       </c>
       <c r="I74" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H75" s="1">
+        <v>150000000</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregar comentarios y ajuste escritura en SQL server, desde clipboard
</commit_message>
<xml_diff>
--- a/Data/Temp/Reporte fidelizaciones Satelite.xlsx
+++ b/Data/Temp/Reporte fidelizaciones Satelite.xlsx
@@ -1343,7 +1343,7 @@
   <dimension ref="A1:KFA76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,7 +1423,7 @@
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>328</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11 7593:7593" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
agregado de nuevos assets
</commit_message>
<xml_diff>
--- a/Data/Temp/Reporte fidelizaciones Satelite.xlsx
+++ b/Data/Temp/Reporte fidelizaciones Satelite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>No. Recibo sin PPC</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>1111</t>
-  </si>
-  <si>
-    <t>10000.0000</t>
   </si>
   <si>
     <t>2022-04-11 09:26:00</t>
@@ -141,7 +138,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +459,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -487,22 +484,22 @@
       <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -511,7 +508,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -519,14 +516,14 @@
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
+      <c r="H3" s="1">
+        <v>10000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>